<commit_message>
update giao dien va mot so tinh nang: Doi mat khau, show danh sach giang vien, Hien thi danh sach hoc vien theo tung dot
</commit_message>
<xml_diff>
--- a/demolist_cnbm.xlsx
+++ b/demolist_cnbm.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DELL\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\UET\KLTN\vnu-portal\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{81C52578-1244-45E4-883D-286513C6607A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2605B7F-2868-43A2-88C5-193927A21B7C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{BFA63368-A593-4B46-AF1E-9436501C34A3}"/>
   </bookViews>
@@ -45,9 +45,6 @@
     <t>cnbm1@vnu.edu.vn</t>
   </si>
   <si>
-    <t>B</t>
-  </si>
-  <si>
     <t>Chủ nhiệm bộ môn 2</t>
   </si>
   <si>
@@ -96,28 +93,31 @@
     <t>cnbm9@vnu.edu.vn</t>
   </si>
   <si>
-    <t>A</t>
-  </si>
-  <si>
-    <t>C</t>
-  </si>
-  <si>
-    <t>D</t>
-  </si>
-  <si>
-    <t>E</t>
-  </si>
-  <si>
-    <t>F</t>
-  </si>
-  <si>
-    <t>G</t>
-  </si>
-  <si>
-    <t>H</t>
-  </si>
-  <si>
-    <t>I</t>
+    <t>Khoa học máy tính</t>
+  </si>
+  <si>
+    <t>Kỹ thuật điện tử</t>
+  </si>
+  <si>
+    <t>Kỹ thuật viễn thông</t>
+  </si>
+  <si>
+    <t>Kỹ thuật xây dựng</t>
+  </si>
+  <si>
+    <t>Vật liệu và linh kiện nano</t>
+  </si>
+  <si>
+    <t>An toàn thông tin</t>
+  </si>
+  <si>
+    <t>Cơ kỹ thuật</t>
+  </si>
+  <si>
+    <t>Kỹ thuật phần mềm</t>
+  </si>
+  <si>
+    <t>Mạng máy tính và truyền thông dữ liệu</t>
   </si>
 </sst>
 </file>
@@ -489,13 +489,14 @@
   <dimension ref="A1:D18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="18.88671875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="32.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
@@ -523,7 +524,7 @@
         <v>5</v>
       </c>
       <c r="D2" t="s">
-        <v>6</v>
+        <v>23</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
@@ -531,13 +532,13 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
@@ -545,10 +546,10 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D4" t="s">
         <v>24</v>
@@ -559,10 +560,10 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D5" t="s">
         <v>25</v>
@@ -573,10 +574,10 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D6" t="s">
         <v>26</v>
@@ -587,10 +588,10 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D7" t="s">
         <v>27</v>
@@ -601,10 +602,10 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D8" t="s">
         <v>28</v>
@@ -615,10 +616,10 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D9" t="s">
         <v>29</v>
@@ -629,10 +630,10 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D10" t="s">
         <v>30</v>

</xml_diff>